<commit_message>
modified the metadata csv file
</commit_message>
<xml_diff>
--- a/Metadata/Somali_Accent_DB_Metadata.xlsx
+++ b/Metadata/Somali_Accent_DB_Metadata.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28605"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\MI2PEPF000005B4\EXCELCNV\d974c8b0-d1aa-4bef-a02c-0ae81a73f1f0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EA17A99-8F6F-4C3F-8911-0B3AF53D94B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{234095A6-81C9-4286-89A2-A878FA94F747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{1670D249-4C3F-47C1-8C14-12B4933AC961}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sheet1!$G$1:$G$192</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -98,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="427">
   <si>
     <t>Speaker_ID</t>
   </si>
@@ -1139,6 +1142,246 @@
   </si>
   <si>
     <t>SOM160_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM161</t>
+  </si>
+  <si>
+    <t>SOM161_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM162</t>
+  </si>
+  <si>
+    <t>SOM162_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM163</t>
+  </si>
+  <si>
+    <t>SOM163_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM164</t>
+  </si>
+  <si>
+    <t>SOM164_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM165</t>
+  </si>
+  <si>
+    <t>SOM165_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM166</t>
+  </si>
+  <si>
+    <t>SOM166_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM167</t>
+  </si>
+  <si>
+    <t>SOM167_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM168</t>
+  </si>
+  <si>
+    <t>SOM168_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM169</t>
+  </si>
+  <si>
+    <t>SOM169_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM170</t>
+  </si>
+  <si>
+    <t>SOM170_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM171</t>
+  </si>
+  <si>
+    <t>SOM171_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM172</t>
+  </si>
+  <si>
+    <t>SOM172_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM173</t>
+  </si>
+  <si>
+    <t>SOM173_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM174</t>
+  </si>
+  <si>
+    <t>SOM174_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM175</t>
+  </si>
+  <si>
+    <t>SOM175_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM176</t>
+  </si>
+  <si>
+    <t>SOM176_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM177</t>
+  </si>
+  <si>
+    <t>SOM177_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM178</t>
+  </si>
+  <si>
+    <t>SOM178_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM179</t>
+  </si>
+  <si>
+    <t>SOM179_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM180</t>
+  </si>
+  <si>
+    <t>SOM180_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM181</t>
+  </si>
+  <si>
+    <t>SOM181_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM182</t>
+  </si>
+  <si>
+    <t>SOM182_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM183</t>
+  </si>
+  <si>
+    <t>SOM183_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM184</t>
+  </si>
+  <si>
+    <t>SOM184_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM185</t>
+  </si>
+  <si>
+    <t>SOM185_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM186</t>
+  </si>
+  <si>
+    <t>SOM186_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM187</t>
+  </si>
+  <si>
+    <t>SOM187_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM188</t>
+  </si>
+  <si>
+    <t>SOM188_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM189</t>
+  </si>
+  <si>
+    <t>SOM189_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM190</t>
+  </si>
+  <si>
+    <t>SOM190_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM191</t>
+  </si>
+  <si>
+    <t>SOM191_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM192</t>
+  </si>
+  <si>
+    <t>SOM192_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM193</t>
+  </si>
+  <si>
+    <t>SOM193_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM194</t>
+  </si>
+  <si>
+    <t>SOM194_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM195</t>
+  </si>
+  <si>
+    <t>SOM195_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM196</t>
+  </si>
+  <si>
+    <t>SOM196_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM197</t>
+  </si>
+  <si>
+    <t>SOM197_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM198</t>
+  </si>
+  <si>
+    <t>SOM198_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM199</t>
+  </si>
+  <si>
+    <t>SOM199_sentence1.wav</t>
+  </si>
+  <si>
+    <t>SOM200</t>
+  </si>
+  <si>
+    <t>SOM200_sentence1.wav</t>
   </si>
 </sst>
 </file>
@@ -3117,10 +3360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60544FB7-22A5-4752-BA5C-F0329FCC1E2A}">
-  <dimension ref="A1:K161"/>
+  <dimension ref="A1:K201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="J162" sqref="J162"/>
+    <sheetView tabSelected="1" topLeftCell="E198" workbookViewId="0">
+      <selection activeCell="J202" sqref="J202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4141,7 +4384,7 @@
         <v>16</v>
       </c>
       <c r="H29" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I29" t="s">
         <v>79</v>
@@ -7011,7 +7254,7 @@
         <v>21</v>
       </c>
       <c r="H111" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I111" t="s">
         <v>17</v>
@@ -8131,7 +8374,7 @@
         <v>195</v>
       </c>
       <c r="H143" s="4">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I143" t="s">
         <v>17</v>
@@ -8586,7 +8829,7 @@
         <v>195</v>
       </c>
       <c r="H156" s="4">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I156" t="s">
         <v>17</v>
@@ -8773,7 +9016,1408 @@
         <v>45697</v>
       </c>
     </row>
+    <row r="162" spans="1:11">
+      <c r="A162" t="s">
+        <v>347</v>
+      </c>
+      <c r="B162" t="s">
+        <v>348</v>
+      </c>
+      <c r="C162" t="s">
+        <v>24</v>
+      </c>
+      <c r="D162" t="s">
+        <v>14</v>
+      </c>
+      <c r="E162" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F162" t="s">
+        <v>15</v>
+      </c>
+      <c r="G162" t="s">
+        <v>195</v>
+      </c>
+      <c r="H162" s="4">
+        <v>29</v>
+      </c>
+      <c r="I162" t="s">
+        <v>17</v>
+      </c>
+      <c r="J162" t="s">
+        <v>142</v>
+      </c>
+      <c r="K162" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11">
+      <c r="A163" t="s">
+        <v>349</v>
+      </c>
+      <c r="B163" t="s">
+        <v>350</v>
+      </c>
+      <c r="C163" t="s">
+        <v>24</v>
+      </c>
+      <c r="D163" t="s">
+        <v>14</v>
+      </c>
+      <c r="E163" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F163" t="s">
+        <v>15</v>
+      </c>
+      <c r="G163" t="s">
+        <v>195</v>
+      </c>
+      <c r="H163" s="4">
+        <v>29</v>
+      </c>
+      <c r="I163" t="s">
+        <v>17</v>
+      </c>
+      <c r="J163" t="s">
+        <v>142</v>
+      </c>
+      <c r="K163" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11">
+      <c r="A164" t="s">
+        <v>351</v>
+      </c>
+      <c r="B164" t="s">
+        <v>352</v>
+      </c>
+      <c r="C164" t="s">
+        <v>24</v>
+      </c>
+      <c r="D164" t="s">
+        <v>14</v>
+      </c>
+      <c r="E164" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F164" t="s">
+        <v>15</v>
+      </c>
+      <c r="G164" t="s">
+        <v>195</v>
+      </c>
+      <c r="H164" s="4">
+        <v>25</v>
+      </c>
+      <c r="I164" t="s">
+        <v>17</v>
+      </c>
+      <c r="J164" t="s">
+        <v>142</v>
+      </c>
+      <c r="K164" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11">
+      <c r="A165" t="s">
+        <v>353</v>
+      </c>
+      <c r="B165" t="s">
+        <v>354</v>
+      </c>
+      <c r="C165" t="s">
+        <v>13</v>
+      </c>
+      <c r="D165" t="s">
+        <v>14</v>
+      </c>
+      <c r="E165" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F165" t="s">
+        <v>15</v>
+      </c>
+      <c r="G165" t="s">
+        <v>208</v>
+      </c>
+      <c r="H165" s="4">
+        <v>33</v>
+      </c>
+      <c r="I165" t="s">
+        <v>17</v>
+      </c>
+      <c r="J165" t="s">
+        <v>142</v>
+      </c>
+      <c r="K165" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11">
+      <c r="A166" t="s">
+        <v>355</v>
+      </c>
+      <c r="B166" t="s">
+        <v>356</v>
+      </c>
+      <c r="C166" t="s">
+        <v>13</v>
+      </c>
+      <c r="D166" t="s">
+        <v>57</v>
+      </c>
+      <c r="E166" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F166" t="s">
+        <v>15</v>
+      </c>
+      <c r="G166" t="s">
+        <v>16</v>
+      </c>
+      <c r="H166" s="4">
+        <v>33</v>
+      </c>
+      <c r="I166" t="s">
+        <v>17</v>
+      </c>
+      <c r="J166" t="s">
+        <v>142</v>
+      </c>
+      <c r="K166" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11">
+      <c r="A167" t="s">
+        <v>357</v>
+      </c>
+      <c r="B167" t="s">
+        <v>358</v>
+      </c>
+      <c r="C167" t="s">
+        <v>13</v>
+      </c>
+      <c r="D167" t="s">
+        <v>14</v>
+      </c>
+      <c r="E167" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F167" t="s">
+        <v>15</v>
+      </c>
+      <c r="G167" t="s">
+        <v>16</v>
+      </c>
+      <c r="H167" s="4">
+        <v>27</v>
+      </c>
+      <c r="I167" t="s">
+        <v>17</v>
+      </c>
+      <c r="J167" t="s">
+        <v>18</v>
+      </c>
+      <c r="K167" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11">
+      <c r="A168" t="s">
+        <v>359</v>
+      </c>
+      <c r="B168" t="s">
+        <v>360</v>
+      </c>
+      <c r="C168" t="s">
+        <v>13</v>
+      </c>
+      <c r="D168" t="s">
+        <v>14</v>
+      </c>
+      <c r="E168" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F168" t="s">
+        <v>15</v>
+      </c>
+      <c r="G168" t="s">
+        <v>16</v>
+      </c>
+      <c r="H168" s="4">
+        <v>36</v>
+      </c>
+      <c r="I168" t="s">
+        <v>17</v>
+      </c>
+      <c r="J168" t="s">
+        <v>142</v>
+      </c>
+      <c r="K168" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11">
+      <c r="A169" t="s">
+        <v>361</v>
+      </c>
+      <c r="B169" t="s">
+        <v>362</v>
+      </c>
+      <c r="C169" t="s">
+        <v>24</v>
+      </c>
+      <c r="D169" t="s">
+        <v>14</v>
+      </c>
+      <c r="E169" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F169" t="s">
+        <v>15</v>
+      </c>
+      <c r="G169" t="s">
+        <v>21</v>
+      </c>
+      <c r="H169" s="4">
+        <v>33</v>
+      </c>
+      <c r="I169" t="s">
+        <v>17</v>
+      </c>
+      <c r="J169" t="s">
+        <v>142</v>
+      </c>
+      <c r="K169" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11">
+      <c r="A170" t="s">
+        <v>363</v>
+      </c>
+      <c r="B170" t="s">
+        <v>364</v>
+      </c>
+      <c r="C170" t="s">
+        <v>24</v>
+      </c>
+      <c r="D170" t="s">
+        <v>14</v>
+      </c>
+      <c r="E170" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F170" t="s">
+        <v>15</v>
+      </c>
+      <c r="G170" t="s">
+        <v>21</v>
+      </c>
+      <c r="H170" s="4">
+        <v>30</v>
+      </c>
+      <c r="I170" t="s">
+        <v>17</v>
+      </c>
+      <c r="J170" t="s">
+        <v>18</v>
+      </c>
+      <c r="K170" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11">
+      <c r="A171" t="s">
+        <v>365</v>
+      </c>
+      <c r="B171" t="s">
+        <v>366</v>
+      </c>
+      <c r="C171" t="s">
+        <v>24</v>
+      </c>
+      <c r="D171" t="s">
+        <v>14</v>
+      </c>
+      <c r="E171" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F171" t="s">
+        <v>15</v>
+      </c>
+      <c r="G171" t="s">
+        <v>208</v>
+      </c>
+      <c r="H171" s="4">
+        <v>37</v>
+      </c>
+      <c r="I171" t="s">
+        <v>17</v>
+      </c>
+      <c r="J171" t="s">
+        <v>18</v>
+      </c>
+      <c r="K171" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11">
+      <c r="A172" t="s">
+        <v>367</v>
+      </c>
+      <c r="B172" t="s">
+        <v>368</v>
+      </c>
+      <c r="C172" t="s">
+        <v>24</v>
+      </c>
+      <c r="D172" t="s">
+        <v>14</v>
+      </c>
+      <c r="E172" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F172" t="s">
+        <v>15</v>
+      </c>
+      <c r="G172" t="s">
+        <v>21</v>
+      </c>
+      <c r="H172" s="4">
+        <v>34</v>
+      </c>
+      <c r="I172" t="s">
+        <v>17</v>
+      </c>
+      <c r="J172" t="s">
+        <v>142</v>
+      </c>
+      <c r="K172" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11">
+      <c r="A173" t="s">
+        <v>369</v>
+      </c>
+      <c r="B173" t="s">
+        <v>370</v>
+      </c>
+      <c r="C173" t="s">
+        <v>13</v>
+      </c>
+      <c r="D173" t="s">
+        <v>14</v>
+      </c>
+      <c r="E173" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F173" t="s">
+        <v>15</v>
+      </c>
+      <c r="G173" t="s">
+        <v>208</v>
+      </c>
+      <c r="H173" s="4">
+        <v>37</v>
+      </c>
+      <c r="I173" t="s">
+        <v>17</v>
+      </c>
+      <c r="J173" t="s">
+        <v>18</v>
+      </c>
+      <c r="K173" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11">
+      <c r="A174" t="s">
+        <v>371</v>
+      </c>
+      <c r="B174" t="s">
+        <v>372</v>
+      </c>
+      <c r="C174" t="s">
+        <v>13</v>
+      </c>
+      <c r="D174" t="s">
+        <v>14</v>
+      </c>
+      <c r="E174" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F174" t="s">
+        <v>15</v>
+      </c>
+      <c r="G174" t="s">
+        <v>21</v>
+      </c>
+      <c r="H174" s="4">
+        <v>32</v>
+      </c>
+      <c r="I174" t="s">
+        <v>17</v>
+      </c>
+      <c r="J174" t="s">
+        <v>18</v>
+      </c>
+      <c r="K174" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11">
+      <c r="A175" t="s">
+        <v>373</v>
+      </c>
+      <c r="B175" t="s">
+        <v>374</v>
+      </c>
+      <c r="C175" t="s">
+        <v>24</v>
+      </c>
+      <c r="D175" t="s">
+        <v>14</v>
+      </c>
+      <c r="E175" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F175" t="s">
+        <v>15</v>
+      </c>
+      <c r="G175" t="s">
+        <v>16</v>
+      </c>
+      <c r="H175" s="4">
+        <v>30</v>
+      </c>
+      <c r="I175" t="s">
+        <v>17</v>
+      </c>
+      <c r="J175" t="s">
+        <v>18</v>
+      </c>
+      <c r="K175" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11">
+      <c r="A176" t="s">
+        <v>375</v>
+      </c>
+      <c r="B176" t="s">
+        <v>376</v>
+      </c>
+      <c r="C176" t="s">
+        <v>24</v>
+      </c>
+      <c r="D176" t="s">
+        <v>14</v>
+      </c>
+      <c r="E176" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F176" t="s">
+        <v>15</v>
+      </c>
+      <c r="G176" t="s">
+        <v>16</v>
+      </c>
+      <c r="H176" s="4">
+        <v>34</v>
+      </c>
+      <c r="I176" t="s">
+        <v>17</v>
+      </c>
+      <c r="J176" t="s">
+        <v>18</v>
+      </c>
+      <c r="K176" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11">
+      <c r="A177" t="s">
+        <v>377</v>
+      </c>
+      <c r="B177" t="s">
+        <v>378</v>
+      </c>
+      <c r="C177" t="s">
+        <v>24</v>
+      </c>
+      <c r="D177" t="s">
+        <v>14</v>
+      </c>
+      <c r="E177" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F177" t="s">
+        <v>15</v>
+      </c>
+      <c r="G177" t="s">
+        <v>16</v>
+      </c>
+      <c r="H177" s="4">
+        <v>41</v>
+      </c>
+      <c r="I177" t="s">
+        <v>17</v>
+      </c>
+      <c r="J177" t="s">
+        <v>142</v>
+      </c>
+      <c r="K177" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11">
+      <c r="A178" t="s">
+        <v>379</v>
+      </c>
+      <c r="B178" t="s">
+        <v>380</v>
+      </c>
+      <c r="C178" t="s">
+        <v>24</v>
+      </c>
+      <c r="D178" t="s">
+        <v>14</v>
+      </c>
+      <c r="E178" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F178" t="s">
+        <v>15</v>
+      </c>
+      <c r="G178" t="s">
+        <v>195</v>
+      </c>
+      <c r="H178" s="4">
+        <v>36</v>
+      </c>
+      <c r="I178" t="s">
+        <v>17</v>
+      </c>
+      <c r="J178" t="s">
+        <v>142</v>
+      </c>
+      <c r="K178" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11">
+      <c r="A179" t="s">
+        <v>381</v>
+      </c>
+      <c r="B179" t="s">
+        <v>382</v>
+      </c>
+      <c r="C179" t="s">
+        <v>24</v>
+      </c>
+      <c r="D179" t="s">
+        <v>14</v>
+      </c>
+      <c r="E179" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F179" t="s">
+        <v>15</v>
+      </c>
+      <c r="G179" t="s">
+        <v>16</v>
+      </c>
+      <c r="H179" s="4">
+        <v>22</v>
+      </c>
+      <c r="I179" t="s">
+        <v>17</v>
+      </c>
+      <c r="J179" t="s">
+        <v>18</v>
+      </c>
+      <c r="K179" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11">
+      <c r="A180" t="s">
+        <v>383</v>
+      </c>
+      <c r="B180" t="s">
+        <v>384</v>
+      </c>
+      <c r="C180" t="s">
+        <v>13</v>
+      </c>
+      <c r="D180" t="s">
+        <v>14</v>
+      </c>
+      <c r="E180" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F180" t="s">
+        <v>15</v>
+      </c>
+      <c r="G180" t="s">
+        <v>16</v>
+      </c>
+      <c r="H180" s="4">
+        <v>26</v>
+      </c>
+      <c r="I180" t="s">
+        <v>17</v>
+      </c>
+      <c r="J180" t="s">
+        <v>18</v>
+      </c>
+      <c r="K180" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11">
+      <c r="A181" t="s">
+        <v>385</v>
+      </c>
+      <c r="B181" t="s">
+        <v>386</v>
+      </c>
+      <c r="C181" t="s">
+        <v>24</v>
+      </c>
+      <c r="D181" t="s">
+        <v>14</v>
+      </c>
+      <c r="E181" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F181" t="s">
+        <v>15</v>
+      </c>
+      <c r="G181" t="s">
+        <v>16</v>
+      </c>
+      <c r="H181" s="4">
+        <v>28</v>
+      </c>
+      <c r="I181" t="s">
+        <v>17</v>
+      </c>
+      <c r="J181" t="s">
+        <v>142</v>
+      </c>
+      <c r="K181" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11">
+      <c r="A182" t="s">
+        <v>387</v>
+      </c>
+      <c r="B182" t="s">
+        <v>388</v>
+      </c>
+      <c r="C182" t="s">
+        <v>24</v>
+      </c>
+      <c r="D182" t="s">
+        <v>14</v>
+      </c>
+      <c r="E182" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F182" t="s">
+        <v>15</v>
+      </c>
+      <c r="G182" t="s">
+        <v>16</v>
+      </c>
+      <c r="H182" s="4">
+        <v>31</v>
+      </c>
+      <c r="I182" t="s">
+        <v>17</v>
+      </c>
+      <c r="J182" t="s">
+        <v>142</v>
+      </c>
+      <c r="K182" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11">
+      <c r="A183" t="s">
+        <v>389</v>
+      </c>
+      <c r="B183" t="s">
+        <v>390</v>
+      </c>
+      <c r="C183" t="s">
+        <v>24</v>
+      </c>
+      <c r="D183" t="s">
+        <v>14</v>
+      </c>
+      <c r="E183" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F183" t="s">
+        <v>15</v>
+      </c>
+      <c r="G183" t="s">
+        <v>208</v>
+      </c>
+      <c r="H183" s="4">
+        <v>31</v>
+      </c>
+      <c r="I183" t="s">
+        <v>17</v>
+      </c>
+      <c r="J183" t="s">
+        <v>142</v>
+      </c>
+      <c r="K183" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11">
+      <c r="A184" t="s">
+        <v>391</v>
+      </c>
+      <c r="B184" t="s">
+        <v>392</v>
+      </c>
+      <c r="C184" t="s">
+        <v>24</v>
+      </c>
+      <c r="D184" t="s">
+        <v>14</v>
+      </c>
+      <c r="E184" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F184" t="s">
+        <v>15</v>
+      </c>
+      <c r="G184" t="s">
+        <v>21</v>
+      </c>
+      <c r="H184" s="4">
+        <v>55</v>
+      </c>
+      <c r="I184" t="s">
+        <v>17</v>
+      </c>
+      <c r="J184" t="s">
+        <v>142</v>
+      </c>
+      <c r="K184" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11">
+      <c r="A185" t="s">
+        <v>393</v>
+      </c>
+      <c r="B185" t="s">
+        <v>394</v>
+      </c>
+      <c r="C185" t="s">
+        <v>13</v>
+      </c>
+      <c r="D185" t="s">
+        <v>14</v>
+      </c>
+      <c r="E185" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F185" t="s">
+        <v>15</v>
+      </c>
+      <c r="G185" t="s">
+        <v>21</v>
+      </c>
+      <c r="H185" s="4">
+        <v>40</v>
+      </c>
+      <c r="I185" t="s">
+        <v>17</v>
+      </c>
+      <c r="J185" t="s">
+        <v>142</v>
+      </c>
+      <c r="K185" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11">
+      <c r="A186" t="s">
+        <v>395</v>
+      </c>
+      <c r="B186" t="s">
+        <v>396</v>
+      </c>
+      <c r="C186" t="s">
+        <v>13</v>
+      </c>
+      <c r="D186" t="s">
+        <v>57</v>
+      </c>
+      <c r="E186" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F186" t="s">
+        <v>15</v>
+      </c>
+      <c r="G186" t="s">
+        <v>16</v>
+      </c>
+      <c r="H186" s="4">
+        <v>28</v>
+      </c>
+      <c r="I186" t="s">
+        <v>17</v>
+      </c>
+      <c r="J186" t="s">
+        <v>18</v>
+      </c>
+      <c r="K186" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11">
+      <c r="A187" t="s">
+        <v>397</v>
+      </c>
+      <c r="B187" t="s">
+        <v>398</v>
+      </c>
+      <c r="C187" t="s">
+        <v>13</v>
+      </c>
+      <c r="D187" t="s">
+        <v>14</v>
+      </c>
+      <c r="E187" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F187" t="s">
+        <v>15</v>
+      </c>
+      <c r="G187" t="s">
+        <v>21</v>
+      </c>
+      <c r="H187" s="4">
+        <v>43</v>
+      </c>
+      <c r="I187" t="s">
+        <v>17</v>
+      </c>
+      <c r="J187" t="s">
+        <v>18</v>
+      </c>
+      <c r="K187" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11">
+      <c r="A188" t="s">
+        <v>399</v>
+      </c>
+      <c r="B188" t="s">
+        <v>400</v>
+      </c>
+      <c r="C188" t="s">
+        <v>13</v>
+      </c>
+      <c r="D188" t="s">
+        <v>14</v>
+      </c>
+      <c r="E188" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F188" t="s">
+        <v>15</v>
+      </c>
+      <c r="G188" t="s">
+        <v>208</v>
+      </c>
+      <c r="H188" s="4">
+        <v>41</v>
+      </c>
+      <c r="I188" t="s">
+        <v>17</v>
+      </c>
+      <c r="J188" t="s">
+        <v>18</v>
+      </c>
+      <c r="K188" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11">
+      <c r="A189" t="s">
+        <v>401</v>
+      </c>
+      <c r="B189" t="s">
+        <v>402</v>
+      </c>
+      <c r="C189" t="s">
+        <v>24</v>
+      </c>
+      <c r="D189" t="s">
+        <v>14</v>
+      </c>
+      <c r="E189" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F189" t="s">
+        <v>15</v>
+      </c>
+      <c r="G189" t="s">
+        <v>195</v>
+      </c>
+      <c r="H189" s="4">
+        <v>30</v>
+      </c>
+      <c r="I189" t="s">
+        <v>17</v>
+      </c>
+      <c r="J189" t="s">
+        <v>142</v>
+      </c>
+      <c r="K189" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11">
+      <c r="A190" t="s">
+        <v>403</v>
+      </c>
+      <c r="B190" t="s">
+        <v>404</v>
+      </c>
+      <c r="C190" t="s">
+        <v>13</v>
+      </c>
+      <c r="D190" t="s">
+        <v>14</v>
+      </c>
+      <c r="E190" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F190" t="s">
+        <v>15</v>
+      </c>
+      <c r="G190" t="s">
+        <v>195</v>
+      </c>
+      <c r="H190" s="4">
+        <v>38</v>
+      </c>
+      <c r="I190" t="s">
+        <v>17</v>
+      </c>
+      <c r="J190" t="s">
+        <v>142</v>
+      </c>
+      <c r="K190" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11">
+      <c r="A191" t="s">
+        <v>405</v>
+      </c>
+      <c r="B191" t="s">
+        <v>406</v>
+      </c>
+      <c r="C191" t="s">
+        <v>13</v>
+      </c>
+      <c r="D191" t="s">
+        <v>14</v>
+      </c>
+      <c r="E191" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F191" t="s">
+        <v>15</v>
+      </c>
+      <c r="G191" t="s">
+        <v>208</v>
+      </c>
+      <c r="H191" s="4">
+        <v>43</v>
+      </c>
+      <c r="I191" t="s">
+        <v>17</v>
+      </c>
+      <c r="J191" t="s">
+        <v>18</v>
+      </c>
+      <c r="K191" s="1">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11">
+      <c r="A192" t="s">
+        <v>407</v>
+      </c>
+      <c r="B192" t="s">
+        <v>408</v>
+      </c>
+      <c r="C192" t="s">
+        <v>13</v>
+      </c>
+      <c r="D192" t="s">
+        <v>14</v>
+      </c>
+      <c r="E192" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F192" t="s">
+        <v>15</v>
+      </c>
+      <c r="G192" t="s">
+        <v>16</v>
+      </c>
+      <c r="H192" s="4">
+        <v>30</v>
+      </c>
+      <c r="I192" t="s">
+        <v>17</v>
+      </c>
+      <c r="J192" t="s">
+        <v>142</v>
+      </c>
+      <c r="K192" s="1">
+        <v>45706</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11">
+      <c r="A193" t="s">
+        <v>409</v>
+      </c>
+      <c r="B193" t="s">
+        <v>410</v>
+      </c>
+      <c r="C193" t="s">
+        <v>13</v>
+      </c>
+      <c r="D193" t="s">
+        <v>14</v>
+      </c>
+      <c r="E193" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F193" t="s">
+        <v>15</v>
+      </c>
+      <c r="G193" t="s">
+        <v>16</v>
+      </c>
+      <c r="H193" s="4">
+        <v>31</v>
+      </c>
+      <c r="I193" t="s">
+        <v>17</v>
+      </c>
+      <c r="J193" t="s">
+        <v>142</v>
+      </c>
+      <c r="K193" s="1">
+        <v>45706</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11">
+      <c r="A194" t="s">
+        <v>411</v>
+      </c>
+      <c r="B194" t="s">
+        <v>412</v>
+      </c>
+      <c r="C194" t="s">
+        <v>13</v>
+      </c>
+      <c r="D194" t="s">
+        <v>14</v>
+      </c>
+      <c r="E194" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F194" t="s">
+        <v>15</v>
+      </c>
+      <c r="G194" t="s">
+        <v>16</v>
+      </c>
+      <c r="H194" s="4">
+        <v>29</v>
+      </c>
+      <c r="I194" t="s">
+        <v>17</v>
+      </c>
+      <c r="J194" t="s">
+        <v>142</v>
+      </c>
+      <c r="K194" s="1">
+        <v>45706</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11">
+      <c r="A195" t="s">
+        <v>413</v>
+      </c>
+      <c r="B195" t="s">
+        <v>414</v>
+      </c>
+      <c r="C195" t="s">
+        <v>24</v>
+      </c>
+      <c r="D195" t="s">
+        <v>14</v>
+      </c>
+      <c r="E195" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F195" t="s">
+        <v>15</v>
+      </c>
+      <c r="G195" t="s">
+        <v>208</v>
+      </c>
+      <c r="H195" s="4">
+        <v>40</v>
+      </c>
+      <c r="I195" t="s">
+        <v>17</v>
+      </c>
+      <c r="J195" t="s">
+        <v>142</v>
+      </c>
+      <c r="K195" s="1">
+        <v>45706</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11">
+      <c r="A196" t="s">
+        <v>415</v>
+      </c>
+      <c r="B196" t="s">
+        <v>416</v>
+      </c>
+      <c r="C196" t="s">
+        <v>24</v>
+      </c>
+      <c r="D196" t="s">
+        <v>14</v>
+      </c>
+      <c r="E196" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F196" t="s">
+        <v>15</v>
+      </c>
+      <c r="G196" t="s">
+        <v>16</v>
+      </c>
+      <c r="H196" s="4">
+        <v>42</v>
+      </c>
+      <c r="I196" t="s">
+        <v>17</v>
+      </c>
+      <c r="J196" t="s">
+        <v>18</v>
+      </c>
+      <c r="K196" s="1">
+        <v>45706</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11">
+      <c r="A197" t="s">
+        <v>417</v>
+      </c>
+      <c r="B197" t="s">
+        <v>418</v>
+      </c>
+      <c r="C197" t="s">
+        <v>13</v>
+      </c>
+      <c r="D197" t="s">
+        <v>14</v>
+      </c>
+      <c r="E197" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F197" t="s">
+        <v>15</v>
+      </c>
+      <c r="G197" t="s">
+        <v>16</v>
+      </c>
+      <c r="H197" s="4">
+        <v>31</v>
+      </c>
+      <c r="I197" t="s">
+        <v>17</v>
+      </c>
+      <c r="J197" t="s">
+        <v>142</v>
+      </c>
+      <c r="K197" s="1">
+        <v>45706</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11">
+      <c r="A198" t="s">
+        <v>419</v>
+      </c>
+      <c r="B198" t="s">
+        <v>420</v>
+      </c>
+      <c r="C198" t="s">
+        <v>13</v>
+      </c>
+      <c r="D198" t="s">
+        <v>14</v>
+      </c>
+      <c r="E198" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F198" t="s">
+        <v>15</v>
+      </c>
+      <c r="G198" t="s">
+        <v>16</v>
+      </c>
+      <c r="H198" s="4">
+        <v>25</v>
+      </c>
+      <c r="I198" t="s">
+        <v>17</v>
+      </c>
+      <c r="J198" t="s">
+        <v>18</v>
+      </c>
+      <c r="K198" s="1">
+        <v>45706</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11">
+      <c r="A199" t="s">
+        <v>421</v>
+      </c>
+      <c r="B199" t="s">
+        <v>422</v>
+      </c>
+      <c r="C199" t="s">
+        <v>13</v>
+      </c>
+      <c r="D199" t="s">
+        <v>14</v>
+      </c>
+      <c r="E199" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F199" t="s">
+        <v>15</v>
+      </c>
+      <c r="G199" t="s">
+        <v>208</v>
+      </c>
+      <c r="H199" s="4">
+        <v>34</v>
+      </c>
+      <c r="I199" t="s">
+        <v>17</v>
+      </c>
+      <c r="J199" t="s">
+        <v>18</v>
+      </c>
+      <c r="K199" s="1">
+        <v>45706</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11">
+      <c r="A200" t="s">
+        <v>423</v>
+      </c>
+      <c r="B200" t="s">
+        <v>424</v>
+      </c>
+      <c r="C200" t="s">
+        <v>13</v>
+      </c>
+      <c r="D200" t="s">
+        <v>14</v>
+      </c>
+      <c r="E200" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F200" t="s">
+        <v>15</v>
+      </c>
+      <c r="G200" t="s">
+        <v>195</v>
+      </c>
+      <c r="H200" s="4">
+        <v>24</v>
+      </c>
+      <c r="I200" t="s">
+        <v>17</v>
+      </c>
+      <c r="J200" t="s">
+        <v>142</v>
+      </c>
+      <c r="K200" s="1">
+        <v>45706</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11">
+      <c r="A201" t="s">
+        <v>425</v>
+      </c>
+      <c r="B201" t="s">
+        <v>426</v>
+      </c>
+      <c r="C201" t="s">
+        <v>13</v>
+      </c>
+      <c r="D201" t="s">
+        <v>14</v>
+      </c>
+      <c r="E201" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F201" t="s">
+        <v>15</v>
+      </c>
+      <c r="G201" t="s">
+        <v>195</v>
+      </c>
+      <c r="H201" s="4">
+        <v>32</v>
+      </c>
+      <c r="I201" t="s">
+        <v>17</v>
+      </c>
+      <c r="J201" t="s">
+        <v>142</v>
+      </c>
+      <c r="K201" s="1">
+        <v>45706</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="G1:G192" xr:uid="{60544FB7-22A5-4752-BA5C-F0329FCC1E2A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>